<commit_message>
time table updated, minor changes
</commit_message>
<xml_diff>
--- a/timeTable.xlsx
+++ b/timeTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samar/Documents/GitHub/Arsd.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78602CF6-EB44-464C-8876-9651FB9A87FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79040E9F-A5A7-8D47-8182-E5D93CF053EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="28240" windowHeight="21720" xr2:uid="{011D48DE-3888-8C47-BFD2-950171D4F5F5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>PERIOD TIME</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>MULTIVARIATE CALCULUS</t>
+  </si>
+  <si>
+    <t>LaTeX and HTML</t>
+  </si>
+  <si>
+    <t>Maxima</t>
   </si>
 </sst>
 </file>
@@ -165,7 +171,7 @@
       <name val="American Typewriter Condensed"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +181,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,6 +214,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -215,46 +233,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,7 +597,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -582,7 +606,8 @@
     <col min="2" max="3" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="4" customWidth="1"/>
     <col min="9" max="10" width="11.5" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="4"/>
   </cols>
@@ -678,11 +703,11 @@
         <v>27</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>27</v>
+      <c r="G4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -691,8 +716,12 @@
       <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="B5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="D5" s="11" t="s">
         <v>29</v>
       </c>
@@ -709,8 +738,12 @@
       <c r="A6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>30</v>
+      </c>
       <c r="D6" s="12" t="s">
         <v>28</v>
       </c>
@@ -727,8 +760,12 @@
       <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="B7" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>30</v>
+      </c>
       <c r="D7" s="12" t="s">
         <v>28</v>
       </c>
@@ -767,8 +804,12 @@
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="B9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="D9" s="12" t="s">
         <v>28</v>
       </c>

</xml_diff>